<commit_message>
Site updated: 2020-02-24 19:05:26
</commit_message>
<xml_diff>
--- a/twogirls/sss.xlsx
+++ b/twogirls/sss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexo\source\twogirls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689970EE-AC2F-43B9-A542-B0D8FDC53F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E029FA92-8C9B-4939-B9F9-A3F3F81B0E46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-504" yWindow="240" windowWidth="16836" windowHeight="10944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="282">
   <si>
     <t xml:space="preserve">  - twogirls/index/1.jpg  </t>
   </si>
@@ -139,6 +139,740 @@
   </si>
   <si>
     <t xml:space="preserve">  - twogirls/index/38.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/39.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/40.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/41.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/42.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/43.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/44.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/45.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/46.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/47.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/48.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/49.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/50.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/51.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/52.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/53.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/54.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/55.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/56.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/57.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/58.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/59.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/60.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/61.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/62.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/63.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/64.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/65.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/66.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/67.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/68.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/69.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/70.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/71.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/72.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/73.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/74.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/75.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/76.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/77.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/78.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/79.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/80.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/81.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/82.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/83.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/84.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/85.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/86.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/87.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/88.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/89.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/90.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/91.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/92.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/93.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/94.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/95.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/96.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/97.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/98.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/99.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/100.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/101.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/102.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/103.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/104.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/105.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/106.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/107.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/108.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/109.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/110.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/111.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/112.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/113.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/114.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/115.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/116.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/117.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/118.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/119.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/120.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/121.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/122.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/123.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/124.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/125.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/126.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/127.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/128.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/129.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/130.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/131.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/132.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/133.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/134.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/135.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/136.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/137.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/138.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/139.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/140.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/141.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/142.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/143.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/144.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/145.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/146.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/147.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/148.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/149.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/150.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/151.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/152.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/153.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/154.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/155.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/156.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/157.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/158.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/159.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/160.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/161.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/162.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/163.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/164.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/165.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/166.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/167.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/168.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/169.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/170.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/171.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/172.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/173.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/174.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/175.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/176.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/177.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/178.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/179.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/180.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/181.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/182.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/183.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/184.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/185.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/186.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/187.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/1.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/2.png</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/7.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/10.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/11.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/12.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/13.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/14.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/15.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/16.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/17.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/18.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/19.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/20.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/21.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/22.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/23.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/24.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/25.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/26.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/27.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/28.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/29.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/30.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/31.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/32.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/33.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/34.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/35.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/36.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/37.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/38.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/39.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/40.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/41.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/42.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/43.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/44.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/45.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/46.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/47.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/48.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/49.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/50.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/51.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/52.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/53.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/54.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/55.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/56.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/57.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/58.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/59.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/60.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/61.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/62.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/63.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/64.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/65.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/66.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/67.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/68.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/69.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/70.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/71.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/72.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/73.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/74.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/75.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/76.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/77.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/78.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/79.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/80.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/81.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/82.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/83.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/84.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/85.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/86.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/87.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/88.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/89.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/90.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/91.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/92.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/93.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/94.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - twogirls/index/95.png</t>
   </si>
 </sst>
 </file>
@@ -472,202 +1206,1298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A38"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91:B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="32.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>